<commit_message>
Se agrega carpeta QA y repote boleta
</commit_message>
<xml_diff>
--- a/Factura Electronica B1i/QA/CasosFEB1i.xlsx
+++ b/Factura Electronica B1i/QA/CasosFEB1i.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>#</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Resultado Esperado</t>
+  </si>
+  <si>
+    <t>Datos Entrada</t>
   </si>
 </sst>
 </file>
@@ -537,282 +540,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F27"/>
+  <dimension ref="B1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="52.85546875" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="6"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="6"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>6</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="8"/>
       <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>9</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>11</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>12</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>13</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>15</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
-      <c r="C18" s="8"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
-      <c r="C19" s="5"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
-      <c r="C20" s="5"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
-      <c r="C21" s="5"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
-      <c r="C22" s="5"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
-      <c r="C23" s="5"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
-      <c r="C24" s="5"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
-      <c r="C25" s="5"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
-      <c r="C26" s="5"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
-      <c r="C27" s="5"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>